<commit_message>
Automatic commit by nbgitpuller
</commit_message>
<xml_diff>
--- a/Results/Battery_Impact factors_results.xlsx
+++ b/Results/Battery_Impact factors_results.xlsx
@@ -251,13 +251,16 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
               <a:t>Global warming potential</a:t>
             </a:r>
           </a:p>
@@ -284,9 +287,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -628,16 +631,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -671,25 +674,37 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t>kg CO2-</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t> Eq</a:t>
                 </a:r>
               </a:p>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US">
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -714,9 +729,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -746,9 +761,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -831,13 +846,16 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
               <a:t>Water use</a:t>
             </a:r>
           </a:p>
@@ -864,9 +882,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1208,16 +1226,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1251,20 +1269,29 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t>m3</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t> world eq. deprived</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US">
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1289,9 +1316,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -1321,9 +1348,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1406,13 +1433,16 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
               <a:t>Acidification</a:t>
             </a:r>
           </a:p>
@@ -1439,9 +1469,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1783,16 +1813,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1826,20 +1856,29 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t>mol H+</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
                   <a:t> Eq</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US">
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1864,9 +1903,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -1981,20 +2020,29 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
               <a:t>Material</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
               <a:t> resources: metals/minerals</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2019,9 +2067,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -2363,16 +2411,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -2406,14 +2454,17 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>kg SB - Eq</a:t>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>kg Sb - Eq</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2439,9 +2490,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -2471,9 +2522,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -5180,8 +5231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="61" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>